<commit_message>
update excel sheet and the description
</commit_message>
<xml_diff>
--- a/neighborhood_comparison/house_price.xlsx
+++ b/neighborhood_comparison/house_price.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo_x\Desktop\Utils\property_project\neighborhood_comparison\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D394036C-756B-4C97-8A3D-94DF02BB1408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="13905" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="HousePrice" sheetId="1" r:id="rId1"/>
+    <sheet name="#ofhousesold" sheetId="2" r:id="rId2"/>
+    <sheet name="Day on Market" sheetId="5" r:id="rId3"/>
+    <sheet name="all info" sheetId="3" r:id="rId4"/>
+    <sheet name="Other potential city" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="146">
   <si>
     <t>City_name</t>
   </si>
@@ -249,24 +247,318 @@
   </si>
   <si>
     <t>Scarsdale</t>
+  </si>
+  <si>
+    <t>Overall Rating</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Housing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Education</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cost of living</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unemployment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commute</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lifestyle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fremont</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oakland</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>San Jose</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Honolulu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP_1st_2022</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP_2nd_2022</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP_3rd_2022</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP_4th_2022</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP_1st_2023</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>change_2023</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>change__2_2022</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>change_3_2022</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>change_4_2022</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arlington</t>
+  </si>
+  <si>
+    <t>Columbus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>San Antonio</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Kansas City</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boise</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idaho</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fort Wayne</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>, Ind.</t>
+  </si>
+  <si>
+    <t>Durham</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Madison</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>, Wisc.</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>St. Petersburg</t>
+  </si>
+  <si>
+    <t>Tampa</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>Colorado Springs</t>
+  </si>
+  <si>
+    <t>Jacksonville</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>Population growth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>employment growth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>increase home value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rental yields</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>San Francisco</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boston</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Washington</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Houston</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seattle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Median monthly rent</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bachelor or higher</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Median income</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Population (thousand)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Housing unit (thousand)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elementary num</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Middle num</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High num</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elementary top rating</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Middle top rating</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>High top rating</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="180" formatCode="0.0_);[Red]\(0.0\)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -290,8 +582,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -352,7 +646,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -387,7 +681,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -564,27 +858,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="AW1" workbookViewId="0">
+      <selection activeCell="BA6" sqref="BA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -781,7 +1076,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -990,7 +1285,7 @@
         <v>395.66666666666669</v>
       </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1150,33 +1445,3796 @@
       <c r="BA3">
         <v>471</v>
       </c>
-    </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.35">
+      <c r="BB3">
+        <f t="shared" ref="BB3:BB6" si="0">SUM(C3:F3)/4</f>
+        <v>365.5</v>
+      </c>
+      <c r="BC3">
+        <f t="shared" ref="BC3:BC6" si="1">SUM(G3:J3)/4</f>
+        <v>384.75</v>
+      </c>
+      <c r="BD3">
+        <f t="shared" ref="BD3:BD6" si="2">SUM(K3:O3)/5</f>
+        <v>464</v>
+      </c>
+      <c r="BE3">
+        <f t="shared" ref="BE3:BE6" si="3">SUM(P3:S3)/4</f>
+        <v>542.5</v>
+      </c>
+      <c r="BF3">
+        <f t="shared" ref="BF3:BF6" si="4">SUM(T3:W3)/4</f>
+        <v>590</v>
+      </c>
+      <c r="BG3">
+        <f t="shared" ref="BG3:BG6" si="5">SUM(X3:AB3)/5</f>
+        <v>568.20000000000005</v>
+      </c>
+      <c r="BH3">
+        <f t="shared" ref="BH3:BH6" si="6">SUM(AC3:AF3)/4</f>
+        <v>540</v>
+      </c>
+      <c r="BI3">
+        <f t="shared" ref="BI3:BI6" si="7">SUM(AG3:AK3)/5</f>
+        <v>504.2</v>
+      </c>
+      <c r="BJ3">
+        <f t="shared" ref="BJ3:BJ6" si="8">SUM(AL3:AO3)/4</f>
+        <v>495.75</v>
+      </c>
+      <c r="BK3">
+        <f t="shared" ref="BK3:BK6" si="9">SUM(AP3:AS3)/4</f>
+        <v>496.25</v>
+      </c>
+      <c r="BL3">
+        <f t="shared" ref="BL3:BL6" si="10">SUM(AT3:AX3)/5</f>
+        <v>488.4</v>
+      </c>
+      <c r="BM3">
+        <f t="shared" ref="BM3:BM6" si="11">SUM(AY3:BA3)/3</f>
+        <v>476.33333333333331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>601</v>
+      </c>
+      <c r="D4">
+        <v>605</v>
+      </c>
+      <c r="E4">
+        <v>607</v>
+      </c>
+      <c r="F4">
+        <v>609</v>
+      </c>
+      <c r="G4">
+        <v>614</v>
+      </c>
+      <c r="H4">
+        <v>620</v>
+      </c>
+      <c r="I4">
+        <v>630</v>
+      </c>
+      <c r="J4">
+        <v>641</v>
+      </c>
+      <c r="K4">
+        <v>647</v>
+      </c>
+      <c r="L4">
+        <v>646</v>
+      </c>
+      <c r="M4">
+        <v>645</v>
+      </c>
+      <c r="N4">
+        <v>646</v>
+      </c>
+      <c r="O4">
+        <v>646</v>
+      </c>
+      <c r="P4">
+        <v>647</v>
+      </c>
+      <c r="Q4">
+        <v>649</v>
+      </c>
+      <c r="R4">
+        <v>650</v>
+      </c>
+      <c r="S4">
+        <v>650</v>
+      </c>
+      <c r="T4">
+        <v>648</v>
+      </c>
+      <c r="U4">
+        <v>644</v>
+      </c>
+      <c r="V4">
+        <v>635</v>
+      </c>
+      <c r="W4">
+        <v>628</v>
+      </c>
+      <c r="X4">
+        <v>626</v>
+      </c>
+      <c r="Y4">
+        <v>625</v>
+      </c>
+      <c r="Z4">
+        <v>623</v>
+      </c>
+      <c r="AA4">
+        <v>623</v>
+      </c>
+      <c r="AB4">
+        <v>623</v>
+      </c>
+      <c r="AC4">
+        <v>624</v>
+      </c>
+      <c r="AD4">
+        <v>621</v>
+      </c>
+      <c r="AE4">
+        <v>619</v>
+      </c>
+      <c r="AF4">
+        <v>620</v>
+      </c>
+      <c r="AG4">
+        <v>622</v>
+      </c>
+      <c r="AH4">
+        <v>624</v>
+      </c>
+      <c r="AI4">
+        <v>628</v>
+      </c>
+      <c r="AJ4">
+        <v>629</v>
+      </c>
+      <c r="AK4">
+        <v>628</v>
+      </c>
+      <c r="AL4">
+        <v>627</v>
+      </c>
+      <c r="AM4">
+        <v>625</v>
+      </c>
+      <c r="AN4">
+        <v>624</v>
+      </c>
+      <c r="AO4">
+        <v>622</v>
+      </c>
+      <c r="AP4">
+        <v>618</v>
+      </c>
+      <c r="AQ4">
+        <v>618</v>
+      </c>
+      <c r="AR4">
+        <v>620</v>
+      </c>
+      <c r="AS4">
+        <v>620</v>
+      </c>
+      <c r="AT4">
+        <v>620</v>
+      </c>
+      <c r="AU4">
+        <v>620</v>
+      </c>
+      <c r="AV4">
+        <v>619</v>
+      </c>
+      <c r="AW4">
+        <v>617</v>
+      </c>
+      <c r="AX4">
+        <v>614</v>
+      </c>
+      <c r="AY4">
+        <v>610</v>
+      </c>
+      <c r="AZ4">
+        <v>609</v>
+      </c>
+      <c r="BA4">
+        <v>608</v>
+      </c>
+      <c r="BB4">
+        <f t="shared" si="0"/>
+        <v>605.5</v>
+      </c>
+      <c r="BC4">
+        <f t="shared" si="1"/>
+        <v>626.25</v>
+      </c>
+      <c r="BD4">
+        <f t="shared" si="2"/>
+        <v>646</v>
+      </c>
+      <c r="BE4">
+        <f t="shared" si="3"/>
+        <v>649</v>
+      </c>
+      <c r="BF4">
+        <f t="shared" si="4"/>
+        <v>638.75</v>
+      </c>
+      <c r="BG4">
+        <f t="shared" si="5"/>
+        <v>624</v>
+      </c>
+      <c r="BH4">
+        <f t="shared" si="6"/>
+        <v>621</v>
+      </c>
+      <c r="BI4">
+        <f t="shared" si="7"/>
+        <v>626.20000000000005</v>
+      </c>
+      <c r="BJ4">
+        <f t="shared" si="8"/>
+        <v>624.5</v>
+      </c>
+      <c r="BK4">
+        <f t="shared" si="9"/>
+        <v>619</v>
+      </c>
+      <c r="BL4">
+        <f t="shared" si="10"/>
+        <v>618</v>
+      </c>
+      <c r="BM4">
+        <f t="shared" si="11"/>
+        <v>609</v>
+      </c>
+    </row>
+    <row r="5" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>379</v>
+      </c>
+      <c r="D5">
+        <v>381</v>
+      </c>
+      <c r="E5">
+        <v>381</v>
+      </c>
+      <c r="F5">
+        <v>383</v>
+      </c>
+      <c r="G5">
+        <v>383</v>
+      </c>
+      <c r="H5">
+        <v>388</v>
+      </c>
+      <c r="I5">
+        <v>394</v>
+      </c>
+      <c r="J5">
+        <v>401</v>
+      </c>
+      <c r="K5">
+        <v>404</v>
+      </c>
+      <c r="L5">
+        <v>408</v>
+      </c>
+      <c r="M5">
+        <v>416</v>
+      </c>
+      <c r="N5">
+        <v>422</v>
+      </c>
+      <c r="O5">
+        <v>426</v>
+      </c>
+      <c r="P5">
+        <v>430</v>
+      </c>
+      <c r="Q5">
+        <v>433</v>
+      </c>
+      <c r="R5">
+        <v>437</v>
+      </c>
+      <c r="S5">
+        <v>438</v>
+      </c>
+      <c r="T5">
+        <v>443</v>
+      </c>
+      <c r="U5">
+        <v>444</v>
+      </c>
+      <c r="V5">
+        <v>443</v>
+      </c>
+      <c r="W5">
+        <v>444</v>
+      </c>
+      <c r="X5">
+        <v>447</v>
+      </c>
+      <c r="Y5">
+        <v>451</v>
+      </c>
+      <c r="Z5">
+        <v>451</v>
+      </c>
+      <c r="AA5">
+        <v>452</v>
+      </c>
+      <c r="AB5">
+        <v>451</v>
+      </c>
+      <c r="AC5">
+        <v>451</v>
+      </c>
+      <c r="AD5">
+        <v>450</v>
+      </c>
+      <c r="AE5">
+        <v>451</v>
+      </c>
+      <c r="AF5">
+        <v>454</v>
+      </c>
+      <c r="AG5">
+        <v>455</v>
+      </c>
+      <c r="AH5">
+        <v>456</v>
+      </c>
+      <c r="AI5">
+        <v>457</v>
+      </c>
+      <c r="AJ5">
+        <v>457</v>
+      </c>
+      <c r="AK5">
+        <v>457</v>
+      </c>
+      <c r="AL5">
+        <v>457</v>
+      </c>
+      <c r="AM5">
+        <v>457</v>
+      </c>
+      <c r="AN5">
+        <v>457</v>
+      </c>
+      <c r="AO5">
+        <v>458</v>
+      </c>
+      <c r="AP5">
+        <v>459</v>
+      </c>
+      <c r="AQ5">
+        <v>460</v>
+      </c>
+      <c r="AR5">
+        <v>461</v>
+      </c>
+      <c r="AS5">
+        <v>462</v>
+      </c>
+      <c r="AT5">
+        <v>463</v>
+      </c>
+      <c r="AU5">
+        <v>462</v>
+      </c>
+      <c r="AV5">
+        <v>463</v>
+      </c>
+      <c r="AW5">
+        <v>462</v>
+      </c>
+      <c r="AX5">
+        <v>462</v>
+      </c>
+      <c r="AY5">
+        <v>462</v>
+      </c>
+      <c r="AZ5">
+        <v>462</v>
+      </c>
+      <c r="BA5">
+        <v>462</v>
+      </c>
+      <c r="BB5">
+        <f t="shared" si="0"/>
+        <v>381</v>
+      </c>
+      <c r="BC5">
+        <f t="shared" si="1"/>
+        <v>391.5</v>
+      </c>
+      <c r="BD5">
+        <f t="shared" si="2"/>
+        <v>415.2</v>
+      </c>
+      <c r="BE5">
+        <f t="shared" si="3"/>
+        <v>434.5</v>
+      </c>
+      <c r="BF5">
+        <f t="shared" si="4"/>
+        <v>443.5</v>
+      </c>
+      <c r="BG5">
+        <f t="shared" si="5"/>
+        <v>450.4</v>
+      </c>
+      <c r="BH5">
+        <f t="shared" si="6"/>
+        <v>451.5</v>
+      </c>
+      <c r="BI5">
+        <f t="shared" si="7"/>
+        <v>456.4</v>
+      </c>
+      <c r="BJ5">
+        <f t="shared" si="8"/>
+        <v>457.25</v>
+      </c>
+      <c r="BK5">
+        <f t="shared" si="9"/>
+        <v>460.5</v>
+      </c>
+      <c r="BL5">
+        <f t="shared" si="10"/>
+        <v>462.4</v>
+      </c>
+      <c r="BM5">
+        <f t="shared" si="11"/>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="6" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
+      </c>
+      <c r="C6">
+        <v>477</v>
+      </c>
+      <c r="D6">
+        <v>480</v>
+      </c>
+      <c r="E6">
+        <v>482</v>
+      </c>
+      <c r="F6">
+        <v>484</v>
+      </c>
+      <c r="G6">
+        <v>487</v>
+      </c>
+      <c r="H6">
+        <v>490</v>
+      </c>
+      <c r="I6">
+        <v>493</v>
+      </c>
+      <c r="J6">
+        <v>497</v>
+      </c>
+      <c r="K6">
+        <v>501</v>
+      </c>
+      <c r="L6">
+        <v>502</v>
+      </c>
+      <c r="M6">
+        <v>504</v>
+      </c>
+      <c r="N6">
+        <v>507</v>
+      </c>
+      <c r="O6">
+        <v>509</v>
+      </c>
+      <c r="P6">
+        <v>510</v>
+      </c>
+      <c r="Q6">
+        <v>510</v>
+      </c>
+      <c r="R6">
+        <v>512</v>
+      </c>
+      <c r="S6">
+        <v>514</v>
+      </c>
+      <c r="T6">
+        <v>514</v>
+      </c>
+      <c r="U6">
+        <v>514</v>
+      </c>
+      <c r="V6">
+        <v>514</v>
+      </c>
+      <c r="W6">
+        <v>512</v>
+      </c>
+      <c r="X6">
+        <v>509</v>
+      </c>
+      <c r="Y6">
+        <v>508</v>
+      </c>
+      <c r="Z6">
+        <v>505</v>
+      </c>
+      <c r="AA6">
+        <v>503</v>
+      </c>
+      <c r="AB6">
+        <v>501</v>
+      </c>
+      <c r="AC6">
+        <v>499</v>
+      </c>
+      <c r="AD6">
+        <v>497</v>
+      </c>
+      <c r="AE6">
+        <v>493</v>
+      </c>
+      <c r="AF6">
+        <v>490</v>
+      </c>
+      <c r="AG6">
+        <v>488</v>
+      </c>
+      <c r="AH6">
+        <v>485</v>
+      </c>
+      <c r="AI6">
+        <v>484</v>
+      </c>
+      <c r="AJ6">
+        <v>483</v>
+      </c>
+      <c r="AK6">
+        <v>484</v>
+      </c>
+      <c r="AL6">
+        <v>485</v>
+      </c>
+      <c r="AM6">
+        <v>487</v>
+      </c>
+      <c r="AN6">
+        <v>486</v>
+      </c>
+      <c r="AO6">
+        <v>485</v>
+      </c>
+      <c r="AP6">
+        <v>483</v>
+      </c>
+      <c r="AQ6">
+        <v>483</v>
+      </c>
+      <c r="AR6">
+        <v>484</v>
+      </c>
+      <c r="AS6">
+        <v>484</v>
+      </c>
+      <c r="AT6">
+        <v>484</v>
+      </c>
+      <c r="AU6">
+        <v>485</v>
+      </c>
+      <c r="AV6">
+        <v>484</v>
+      </c>
+      <c r="AW6">
+        <v>483</v>
+      </c>
+      <c r="AX6">
+        <v>482</v>
+      </c>
+      <c r="AY6">
+        <v>483</v>
+      </c>
+      <c r="AZ6">
+        <v>484</v>
+      </c>
+      <c r="BA6">
+        <v>484</v>
+      </c>
+      <c r="BB6">
+        <f t="shared" si="0"/>
+        <v>480.75</v>
+      </c>
+      <c r="BC6">
+        <f t="shared" si="1"/>
+        <v>491.75</v>
+      </c>
+      <c r="BD6">
+        <f t="shared" si="2"/>
+        <v>504.6</v>
+      </c>
+      <c r="BE6">
+        <f t="shared" si="3"/>
+        <v>511.5</v>
+      </c>
+      <c r="BF6">
+        <f t="shared" si="4"/>
+        <v>513.5</v>
+      </c>
+      <c r="BG6">
+        <f t="shared" si="5"/>
+        <v>505.2</v>
+      </c>
+      <c r="BH6">
+        <f t="shared" si="6"/>
+        <v>494.75</v>
+      </c>
+      <c r="BI6">
+        <f t="shared" si="7"/>
+        <v>484.8</v>
+      </c>
+      <c r="BJ6">
+        <f t="shared" si="8"/>
+        <v>485.75</v>
+      </c>
+      <c r="BK6">
+        <f t="shared" si="9"/>
+        <v>483.5</v>
+      </c>
+      <c r="BL6">
+        <f t="shared" si="10"/>
+        <v>483.6</v>
+      </c>
+      <c r="BM6">
+        <f t="shared" si="11"/>
+        <v>483.66666666666669</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>43831</v>
+      </c>
+      <c r="D1" s="1">
+        <v>43862</v>
+      </c>
+      <c r="E1" s="1">
+        <v>43891</v>
+      </c>
+      <c r="F1" s="1">
+        <v>43922</v>
+      </c>
+      <c r="G1" s="1">
+        <v>43952</v>
+      </c>
+      <c r="H1" s="1">
+        <v>43983</v>
+      </c>
+      <c r="I1" s="1">
+        <v>44013</v>
+      </c>
+      <c r="J1" s="1">
+        <v>44044</v>
+      </c>
+      <c r="K1" s="1">
+        <v>44075</v>
+      </c>
+      <c r="L1" s="1">
+        <v>44105</v>
+      </c>
+      <c r="M1" s="1">
+        <v>44136</v>
+      </c>
+      <c r="N1" s="1">
+        <v>44166</v>
+      </c>
+      <c r="O1" s="1">
+        <v>44197</v>
+      </c>
+      <c r="P1" s="1">
+        <v>44228</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>44256</v>
+      </c>
+      <c r="R1" s="1">
+        <v>44287</v>
+      </c>
+      <c r="S1" s="1">
+        <v>44317</v>
+      </c>
+      <c r="T1" s="1">
+        <v>44348</v>
+      </c>
+      <c r="U1" s="1">
+        <v>44378</v>
+      </c>
+      <c r="V1" s="1">
+        <v>44409</v>
+      </c>
+      <c r="W1" s="1">
+        <v>44440</v>
+      </c>
+      <c r="X1" s="1">
+        <v>44470</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>44501</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>44531</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>44562</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>44593</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>44621</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>44652</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>44682</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>44713</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>44743</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>44774</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>44805</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>44835</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>44896</v>
+      </c>
+      <c r="AM1" s="1"/>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>24</v>
+      </c>
+      <c r="I2">
+        <v>12</v>
+      </c>
+      <c r="J2">
+        <v>25</v>
+      </c>
+      <c r="K2">
+        <v>36</v>
+      </c>
+      <c r="L2">
+        <v>22</v>
+      </c>
+      <c r="M2">
+        <v>17</v>
+      </c>
+      <c r="N2">
+        <v>15</v>
+      </c>
+      <c r="O2">
+        <v>13</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+      <c r="Q2">
+        <v>10</v>
+      </c>
+      <c r="R2">
+        <v>9</v>
+      </c>
+      <c r="S2">
+        <v>13</v>
+      </c>
+      <c r="T2">
+        <v>21</v>
+      </c>
+      <c r="U2">
+        <v>31</v>
+      </c>
+      <c r="V2">
+        <v>24</v>
+      </c>
+      <c r="W2">
+        <v>11</v>
+      </c>
+      <c r="X2">
+        <v>6</v>
+      </c>
+      <c r="Y2">
+        <v>10</v>
+      </c>
+      <c r="Z2">
+        <v>13</v>
+      </c>
+      <c r="AA2">
+        <v>10</v>
+      </c>
+      <c r="AB2">
+        <v>4</v>
+      </c>
+      <c r="AC2">
+        <v>9</v>
+      </c>
+      <c r="AD2">
+        <v>13</v>
+      </c>
+      <c r="AE2">
+        <v>14</v>
+      </c>
+      <c r="AF2">
+        <v>11</v>
+      </c>
+      <c r="AG2">
+        <v>18</v>
+      </c>
+      <c r="AH2">
+        <v>22</v>
+      </c>
+      <c r="AI2">
+        <v>11</v>
+      </c>
+      <c r="AJ2">
+        <v>13</v>
+      </c>
+      <c r="AK2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>14</v>
+      </c>
+      <c r="K3">
+        <v>11</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3">
+        <v>8</v>
+      </c>
+      <c r="N3">
+        <v>7</v>
+      </c>
+      <c r="O3">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>9</v>
+      </c>
+      <c r="S3">
+        <v>4</v>
+      </c>
+      <c r="T3">
+        <v>10</v>
+      </c>
+      <c r="U3">
+        <v>9</v>
+      </c>
+      <c r="V3">
+        <v>9</v>
+      </c>
+      <c r="W3">
+        <v>2</v>
+      </c>
+      <c r="X3">
+        <v>7</v>
+      </c>
+      <c r="Y3">
+        <v>9</v>
+      </c>
+      <c r="Z3">
+        <v>10</v>
+      </c>
+      <c r="AA3">
+        <v>7</v>
+      </c>
+      <c r="AB3">
+        <v>2</v>
+      </c>
+      <c r="AC3">
+        <v>4</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>4</v>
+      </c>
+      <c r="AF3">
+        <v>6</v>
+      </c>
+      <c r="AG3">
+        <v>8</v>
+      </c>
+      <c r="AH3">
+        <v>5</v>
+      </c>
+      <c r="AI3">
+        <v>6</v>
+      </c>
+      <c r="AJ3">
+        <v>8</v>
+      </c>
+      <c r="AK3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>27</v>
+      </c>
+      <c r="H4">
+        <v>18</v>
+      </c>
+      <c r="I4">
+        <v>21</v>
+      </c>
+      <c r="J4">
+        <v>30</v>
+      </c>
+      <c r="K4">
+        <v>41</v>
+      </c>
+      <c r="L4">
+        <v>23</v>
+      </c>
+      <c r="M4">
+        <v>25</v>
+      </c>
+      <c r="N4">
+        <v>27</v>
+      </c>
+      <c r="O4">
+        <v>22</v>
+      </c>
+      <c r="P4">
+        <v>16</v>
+      </c>
+      <c r="Q4">
+        <v>19</v>
+      </c>
+      <c r="R4">
+        <v>28</v>
+      </c>
+      <c r="S4">
+        <v>18</v>
+      </c>
+      <c r="T4">
+        <v>43</v>
+      </c>
+      <c r="U4">
+        <v>34</v>
+      </c>
+      <c r="V4">
+        <v>38</v>
+      </c>
+      <c r="W4">
+        <v>25</v>
+      </c>
+      <c r="X4">
+        <v>20</v>
+      </c>
+      <c r="Y4">
+        <v>13</v>
+      </c>
+      <c r="Z4">
+        <v>16</v>
+      </c>
+      <c r="AA4">
+        <v>13</v>
+      </c>
+      <c r="AB4">
+        <v>15</v>
+      </c>
+      <c r="AC4">
+        <v>22</v>
+      </c>
+      <c r="AD4">
+        <v>26</v>
+      </c>
+      <c r="AE4">
+        <v>25</v>
+      </c>
+      <c r="AF4">
+        <v>37</v>
+      </c>
+      <c r="AG4">
+        <v>39</v>
+      </c>
+      <c r="AH4">
+        <v>35</v>
+      </c>
+      <c r="AI4">
+        <v>19</v>
+      </c>
+      <c r="AJ4">
+        <v>14</v>
+      </c>
+      <c r="AK4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <v>31</v>
+      </c>
+      <c r="H6">
+        <v>33</v>
+      </c>
+      <c r="I6">
+        <v>47</v>
+      </c>
+      <c r="J6">
+        <v>72</v>
+      </c>
+      <c r="K6">
+        <v>52</v>
+      </c>
+      <c r="L6">
+        <v>52</v>
+      </c>
+      <c r="M6">
+        <v>44</v>
+      </c>
+      <c r="N6">
+        <v>62</v>
+      </c>
+      <c r="O6">
+        <v>40</v>
+      </c>
+      <c r="P6">
+        <v>40</v>
+      </c>
+      <c r="Q6">
+        <v>35</v>
+      </c>
+      <c r="R6">
+        <v>55</v>
+      </c>
+      <c r="S6">
+        <v>44</v>
+      </c>
+      <c r="T6">
+        <v>56</v>
+      </c>
+      <c r="U6">
+        <v>89</v>
+      </c>
+      <c r="V6">
+        <v>95</v>
+      </c>
+      <c r="W6">
+        <v>37</v>
+      </c>
+      <c r="X6">
+        <v>30</v>
+      </c>
+      <c r="Y6">
+        <v>27</v>
+      </c>
+      <c r="Z6">
+        <v>37</v>
+      </c>
+      <c r="AA6">
+        <v>26</v>
+      </c>
+      <c r="AB6">
+        <v>28</v>
+      </c>
+      <c r="AC6">
+        <v>24</v>
+      </c>
+      <c r="AD6">
+        <v>37</v>
+      </c>
+      <c r="AE6">
+        <v>43</v>
+      </c>
+      <c r="AF6">
+        <v>69</v>
+      </c>
+      <c r="AG6">
+        <v>65</v>
+      </c>
+      <c r="AH6">
+        <v>76</v>
+      </c>
+      <c r="AI6">
+        <v>55</v>
+      </c>
+      <c r="AJ6">
+        <v>27</v>
+      </c>
+      <c r="AK6">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>43831</v>
+      </c>
+      <c r="D1" s="1">
+        <v>43862</v>
+      </c>
+      <c r="E1" s="1">
+        <v>43891</v>
+      </c>
+      <c r="F1" s="1">
+        <v>43922</v>
+      </c>
+      <c r="G1" s="1">
+        <v>43952</v>
+      </c>
+      <c r="H1" s="1">
+        <v>43983</v>
+      </c>
+      <c r="I1" s="1">
+        <v>44013</v>
+      </c>
+      <c r="J1" s="1">
+        <v>44044</v>
+      </c>
+      <c r="K1" s="1">
+        <v>44075</v>
+      </c>
+      <c r="L1" s="1">
+        <v>44105</v>
+      </c>
+      <c r="M1" s="1">
+        <v>44136</v>
+      </c>
+      <c r="N1" s="1">
+        <v>44166</v>
+      </c>
+      <c r="O1" s="1">
+        <v>44197</v>
+      </c>
+      <c r="P1" s="1">
+        <v>44228</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>44256</v>
+      </c>
+      <c r="R1" s="1">
+        <v>44287</v>
+      </c>
+      <c r="S1" s="1">
+        <v>44317</v>
+      </c>
+      <c r="T1" s="1">
+        <v>44348</v>
+      </c>
+      <c r="U1" s="1">
+        <v>44378</v>
+      </c>
+      <c r="V1" s="1">
+        <v>44409</v>
+      </c>
+      <c r="W1" s="1">
+        <v>44440</v>
+      </c>
+      <c r="X1" s="1">
+        <v>44470</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>44501</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>44531</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>44562</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>44593</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>44621</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>44652</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>44682</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>44713</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>44743</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>44774</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>44805</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>44835</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>44866</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>44896</v>
+      </c>
+      <c r="AM1" s="1"/>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>85</v>
+      </c>
+      <c r="D2">
+        <v>59</v>
+      </c>
+      <c r="E2">
+        <v>175</v>
+      </c>
+      <c r="F2">
+        <v>130</v>
+      </c>
+      <c r="G2">
+        <v>32</v>
+      </c>
+      <c r="H2">
+        <v>47</v>
+      </c>
+      <c r="I2">
+        <v>104</v>
+      </c>
+      <c r="J2">
+        <v>74</v>
+      </c>
+      <c r="K2">
+        <v>21</v>
+      </c>
+      <c r="L2">
+        <v>46</v>
+      </c>
+      <c r="M2">
+        <v>29</v>
+      </c>
+      <c r="N2">
+        <v>30</v>
+      </c>
+      <c r="O2">
+        <v>40</v>
+      </c>
+      <c r="P2">
+        <v>64</v>
+      </c>
+      <c r="Q2">
+        <v>74</v>
+      </c>
+      <c r="R2">
+        <v>17</v>
+      </c>
+      <c r="S2">
+        <v>41</v>
+      </c>
+      <c r="T2">
+        <v>16</v>
+      </c>
+      <c r="U2">
+        <v>15</v>
+      </c>
+      <c r="V2">
+        <v>19</v>
+      </c>
+      <c r="W2">
+        <v>21</v>
+      </c>
+      <c r="X2">
+        <v>28</v>
+      </c>
+      <c r="Y2">
+        <v>54</v>
+      </c>
+      <c r="Z2">
+        <v>25</v>
+      </c>
+      <c r="AA2">
+        <v>26</v>
+      </c>
+      <c r="AB2">
+        <v>40</v>
+      </c>
+      <c r="AC2">
+        <v>28</v>
+      </c>
+      <c r="AD2">
+        <v>11</v>
+      </c>
+      <c r="AE2">
+        <v>10</v>
+      </c>
+      <c r="AF2">
+        <v>16</v>
+      </c>
+      <c r="AG2">
+        <v>15</v>
+      </c>
+      <c r="AH2">
+        <v>10</v>
+      </c>
+      <c r="AI2">
+        <v>19</v>
+      </c>
+      <c r="AJ2">
+        <v>21</v>
+      </c>
+      <c r="AK2">
+        <v>21</v>
+      </c>
+      <c r="AL2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>218</v>
+      </c>
+      <c r="D3">
+        <v>61</v>
+      </c>
+      <c r="E3">
+        <v>119</v>
+      </c>
+      <c r="F3">
+        <v>107</v>
+      </c>
+      <c r="G3">
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <v>96</v>
+      </c>
+      <c r="I3">
+        <v>128</v>
+      </c>
+      <c r="J3">
+        <v>47</v>
+      </c>
+      <c r="K3">
+        <v>25</v>
+      </c>
+      <c r="L3">
+        <v>49</v>
+      </c>
+      <c r="M3">
+        <v>71</v>
+      </c>
+      <c r="N3">
+        <v>28</v>
+      </c>
+      <c r="O3">
+        <v>74</v>
+      </c>
+      <c r="P3">
+        <v>70</v>
+      </c>
+      <c r="Q3">
+        <v>79</v>
+      </c>
+      <c r="R3">
+        <v>104</v>
+      </c>
+      <c r="S3">
+        <v>124</v>
+      </c>
+      <c r="T3">
+        <v>87</v>
+      </c>
+      <c r="U3">
+        <v>21</v>
+      </c>
+      <c r="V3">
+        <v>41</v>
+      </c>
+      <c r="W3">
+        <v>46</v>
+      </c>
+      <c r="X3">
+        <v>36</v>
+      </c>
+      <c r="Y3">
+        <v>83</v>
+      </c>
+      <c r="Z3">
+        <v>31</v>
+      </c>
+      <c r="AA3">
+        <v>75</v>
+      </c>
+      <c r="AB3">
+        <v>252</v>
+      </c>
+      <c r="AC3">
+        <v>55</v>
+      </c>
+      <c r="AD3">
+        <v>13</v>
+      </c>
+      <c r="AE3">
+        <v>16</v>
+      </c>
+      <c r="AF3">
+        <v>18</v>
+      </c>
+      <c r="AG3">
+        <v>14</v>
+      </c>
+      <c r="AH3">
+        <v>23</v>
+      </c>
+      <c r="AI3">
+        <v>17</v>
+      </c>
+      <c r="AJ3">
+        <v>28</v>
+      </c>
+      <c r="AK3">
+        <v>28</v>
+      </c>
+      <c r="AL3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>165</v>
+      </c>
+      <c r="D4">
+        <v>74</v>
+      </c>
+      <c r="E4">
+        <v>54</v>
+      </c>
+      <c r="F4">
+        <v>40</v>
+      </c>
+      <c r="G4">
+        <v>66</v>
+      </c>
+      <c r="H4">
+        <v>33</v>
+      </c>
+      <c r="I4">
+        <v>98</v>
+      </c>
+      <c r="J4">
+        <v>19</v>
+      </c>
+      <c r="K4">
+        <v>31</v>
+      </c>
+      <c r="L4">
+        <v>29</v>
+      </c>
+      <c r="M4">
+        <v>68</v>
+      </c>
+      <c r="N4">
+        <v>28</v>
+      </c>
+      <c r="O4">
+        <v>28</v>
+      </c>
+      <c r="P4">
+        <v>65</v>
+      </c>
+      <c r="Q4">
+        <v>43</v>
+      </c>
+      <c r="R4">
+        <v>41</v>
+      </c>
+      <c r="S4">
+        <v>115</v>
+      </c>
+      <c r="T4">
+        <v>21</v>
+      </c>
+      <c r="U4">
+        <v>39</v>
+      </c>
+      <c r="V4">
+        <v>32</v>
+      </c>
+      <c r="W4">
+        <v>31</v>
+      </c>
+      <c r="X4">
+        <v>35</v>
+      </c>
+      <c r="Y4">
+        <v>58</v>
+      </c>
+      <c r="Z4">
+        <v>52</v>
+      </c>
+      <c r="AA4">
+        <v>48</v>
+      </c>
+      <c r="AB4">
+        <v>89</v>
+      </c>
+      <c r="AC4">
+        <v>86</v>
+      </c>
+      <c r="AD4">
+        <v>13</v>
+      </c>
+      <c r="AE4">
+        <v>10</v>
+      </c>
+      <c r="AF4">
+        <v>11</v>
+      </c>
+      <c r="AG4">
+        <v>12</v>
+      </c>
+      <c r="AH4">
+        <v>19</v>
+      </c>
+      <c r="AI4">
+        <v>20</v>
+      </c>
+      <c r="AJ4">
+        <v>54</v>
+      </c>
+      <c r="AK4">
+        <v>25</v>
+      </c>
+      <c r="AL4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>84</v>
+      </c>
+      <c r="D6">
+        <v>115</v>
+      </c>
+      <c r="E6">
+        <v>87</v>
+      </c>
+      <c r="F6">
+        <v>61</v>
+      </c>
+      <c r="G6">
+        <v>33</v>
+      </c>
+      <c r="H6">
+        <v>59</v>
+      </c>
+      <c r="I6">
+        <v>90</v>
+      </c>
+      <c r="J6">
+        <v>35</v>
+      </c>
+      <c r="K6">
+        <v>28</v>
+      </c>
+      <c r="L6">
+        <v>34</v>
+      </c>
+      <c r="M6">
+        <v>52</v>
+      </c>
+      <c r="N6">
+        <v>42</v>
+      </c>
+      <c r="O6">
+        <v>35</v>
+      </c>
+      <c r="P6">
+        <v>54</v>
+      </c>
+      <c r="Q6">
+        <v>41</v>
+      </c>
+      <c r="R6">
+        <v>44</v>
+      </c>
+      <c r="S6">
+        <v>49</v>
+      </c>
+      <c r="T6">
+        <v>18</v>
+      </c>
+      <c r="U6">
+        <v>20</v>
+      </c>
+      <c r="V6">
+        <v>17</v>
+      </c>
+      <c r="W6">
+        <v>22</v>
+      </c>
+      <c r="X6">
+        <v>30</v>
+      </c>
+      <c r="Y6">
+        <v>68</v>
+      </c>
+      <c r="Z6">
+        <v>45</v>
+      </c>
+      <c r="AA6">
+        <v>77</v>
+      </c>
+      <c r="AB6">
+        <v>99</v>
+      </c>
+      <c r="AC6">
+        <v>34</v>
+      </c>
+      <c r="AD6">
+        <v>21</v>
+      </c>
+      <c r="AE6">
+        <v>19</v>
+      </c>
+      <c r="AF6">
+        <v>14</v>
+      </c>
+      <c r="AG6">
+        <v>16</v>
+      </c>
+      <c r="AH6">
+        <v>17</v>
+      </c>
+      <c r="AI6">
+        <v>24</v>
+      </c>
+      <c r="AJ6">
+        <v>56</v>
+      </c>
+      <c r="AK6">
+        <v>30</v>
+      </c>
+      <c r="AL6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AC16" sqref="AC16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>76</v>
+      </c>
+      <c r="R1" t="s">
+        <v>77</v>
+      </c>
+      <c r="S1" t="s">
+        <v>136</v>
+      </c>
+      <c r="T1" t="s">
+        <v>135</v>
+      </c>
+      <c r="U1" t="s">
+        <v>139</v>
+      </c>
+      <c r="V1" t="s">
+        <v>137</v>
+      </c>
+      <c r="W1" t="s">
+        <v>138</v>
+      </c>
+      <c r="X1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>398</v>
+      </c>
+      <c r="D2">
+        <v>410</v>
+      </c>
+      <c r="E2">
+        <v>410</v>
+      </c>
+      <c r="F2">
+        <v>393</v>
+      </c>
+      <c r="G2">
+        <v>399</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>-4.1000000000000005</v>
+      </c>
+      <c r="K2">
+        <v>1.5</v>
+      </c>
+      <c r="L2">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>8</v>
+      </c>
+      <c r="N2">
+        <v>7</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>9</v>
+      </c>
+      <c r="Q2">
+        <v>7</v>
+      </c>
+      <c r="R2">
+        <v>4</v>
+      </c>
+      <c r="S2">
+        <v>87.8</v>
+      </c>
+      <c r="T2">
+        <v>1933</v>
+      </c>
+      <c r="U2">
+        <v>0.5</v>
+      </c>
+      <c r="V2">
+        <v>219804</v>
+      </c>
+      <c r="W2">
+        <v>1.3</v>
+      </c>
+      <c r="X2">
+        <v>8.5</v>
+      </c>
+      <c r="Y2">
+        <v>2</v>
+      </c>
+      <c r="Z2">
+        <v>9</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>364</v>
+      </c>
+      <c r="D3">
+        <v>537</v>
+      </c>
+      <c r="E3">
+        <v>543</v>
+      </c>
+      <c r="F3">
+        <v>497</v>
+      </c>
+      <c r="G3">
+        <v>471</v>
+      </c>
+      <c r="H3">
+        <v>47.5</v>
+      </c>
+      <c r="I3">
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="J3">
+        <v>-8.5</v>
+      </c>
+      <c r="K3">
+        <v>-5.2</v>
+      </c>
+      <c r="L3">
+        <v>9</v>
+      </c>
+      <c r="M3">
+        <v>7</v>
+      </c>
+      <c r="N3">
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>12</v>
+      </c>
+      <c r="Q3">
+        <v>5</v>
+      </c>
+      <c r="R3">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="U3">
+        <v>0.8</v>
+      </c>
+      <c r="V3">
+        <v>259764</v>
+      </c>
+      <c r="W3">
+        <v>1.9</v>
+      </c>
+      <c r="X3">
+        <v>6</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>5</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>6</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>607</v>
+      </c>
+      <c r="D4">
+        <v>649</v>
+      </c>
+      <c r="E4">
+        <v>621</v>
+      </c>
+      <c r="F4">
+        <v>620</v>
+      </c>
+      <c r="G4">
+        <v>608</v>
+      </c>
+      <c r="H4">
+        <v>6.9</v>
+      </c>
+      <c r="I4">
+        <v>-4.3</v>
+      </c>
+      <c r="J4">
+        <v>-0.2</v>
+      </c>
+      <c r="K4">
+        <v>-1.9</v>
+      </c>
+      <c r="L4">
+        <v>9</v>
+      </c>
+      <c r="M4">
+        <v>8</v>
+      </c>
+      <c r="N4">
+        <v>8</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>10</v>
+      </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
+      <c r="R4">
+        <v>6</v>
+      </c>
+      <c r="S4">
+        <v>73.5</v>
+      </c>
+      <c r="T4">
+        <v>2137</v>
+      </c>
+      <c r="U4">
+        <v>5.7</v>
+      </c>
+      <c r="V4">
+        <v>276177</v>
+      </c>
+      <c r="W4">
+        <v>16</v>
+      </c>
+      <c r="X4">
+        <f>(10+9+8+8)/4</f>
+        <v>8.75</v>
+      </c>
+      <c r="Y4">
+        <v>4</v>
+      </c>
+      <c r="Z4">
+        <v>6.5</v>
+      </c>
+      <c r="AA4">
+        <v>2</v>
+      </c>
+      <c r="AB4">
+        <v>8</v>
+      </c>
+      <c r="AC4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>381</v>
+      </c>
+      <c r="D5">
+        <v>433</v>
+      </c>
+      <c r="E5">
+        <v>450</v>
+      </c>
+      <c r="F5">
+        <v>461</v>
+      </c>
+      <c r="G5">
+        <v>462</v>
+      </c>
+      <c r="H5">
+        <v>13.600000000000001</v>
+      </c>
+      <c r="I5">
+        <v>3.9</v>
+      </c>
+      <c r="J5">
+        <v>2.4</v>
+      </c>
+      <c r="K5">
+        <v>0.2</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <v>5</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>8</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5">
+        <v>6</v>
+      </c>
+      <c r="U5">
+        <v>0.8</v>
+      </c>
+      <c r="V5">
+        <v>188685</v>
+      </c>
+      <c r="W5">
+        <v>6.4</v>
+      </c>
+      <c r="X5">
+        <v>8</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>5</v>
+      </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>482</v>
+      </c>
+      <c r="D6">
+        <v>510</v>
+      </c>
+      <c r="E6">
+        <v>497</v>
+      </c>
+      <c r="F6">
+        <v>484</v>
+      </c>
+      <c r="G6">
+        <v>484</v>
+      </c>
+      <c r="H6">
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="I6">
+        <v>-2.5</v>
+      </c>
+      <c r="J6">
+        <v>-2.6</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="M6">
+        <v>8</v>
+      </c>
+      <c r="N6">
+        <v>8</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>11</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <v>6</v>
+      </c>
+      <c r="S6">
+        <v>89</v>
+      </c>
+      <c r="T6">
+        <v>3087</v>
+      </c>
+      <c r="U6">
+        <v>5.8</v>
+      </c>
+      <c r="V6">
+        <v>417335</v>
+      </c>
+      <c r="W6">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="X6">
+        <f>(10+10+8+8+7)/5</f>
+        <v>8.6</v>
+      </c>
+      <c r="Y6">
+        <v>10</v>
+      </c>
+      <c r="Z6">
+        <v>6.5</v>
+      </c>
+      <c r="AA6">
+        <v>4</v>
+      </c>
+      <c r="AB6" s="2">
+        <f>25/3</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="AC6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7">
+        <v>897</v>
+      </c>
+      <c r="D7">
+        <v>933</v>
+      </c>
+      <c r="E7">
+        <v>961</v>
+      </c>
+      <c r="F7">
+        <v>939</v>
+      </c>
+      <c r="G7">
+        <v>903</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="K7">
+        <v>-3.8</v>
+      </c>
+      <c r="L7">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <v>9</v>
+      </c>
+      <c r="N7">
+        <v>10</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>10</v>
+      </c>
+      <c r="Q7">
+        <v>8</v>
+      </c>
+      <c r="R7">
+        <v>10</v>
+      </c>
+      <c r="S7">
+        <v>55.1</v>
+      </c>
+      <c r="T7">
+        <v>2028</v>
+      </c>
+      <c r="U7">
+        <v>76.5</v>
+      </c>
+      <c r="V7">
+        <v>143043</v>
+      </c>
+      <c r="W7">
+        <v>231</v>
+      </c>
+      <c r="X7">
+        <v>9</v>
+      </c>
+      <c r="Y7">
+        <v>50</v>
+      </c>
+      <c r="Z7">
+        <f>(10+9+9+8+7)/5</f>
+        <v>8.6</v>
+      </c>
+      <c r="AA7">
+        <v>18</v>
+      </c>
+      <c r="AB7">
+        <v>8</v>
+      </c>
+      <c r="AC7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8">
+        <v>562</v>
+      </c>
+      <c r="D8">
+        <v>574</v>
+      </c>
+      <c r="E8">
+        <v>591</v>
+      </c>
+      <c r="F8">
+        <v>577</v>
+      </c>
+      <c r="G8">
+        <v>562</v>
+      </c>
+      <c r="H8">
+        <v>2.1</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>-2.4</v>
+      </c>
+      <c r="K8">
+        <v>-2.6</v>
+      </c>
+      <c r="L8">
+        <v>9</v>
+      </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="N8">
+        <v>7</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>6</v>
+      </c>
+      <c r="Q8">
+        <v>11</v>
+      </c>
+      <c r="R8">
+        <v>11</v>
+      </c>
+      <c r="S8">
+        <v>40.6</v>
+      </c>
+      <c r="T8">
+        <v>1255</v>
+      </c>
+      <c r="U8">
+        <v>169.3</v>
+      </c>
+      <c r="V8">
+        <v>93849</v>
+      </c>
+      <c r="W8">
+        <v>417.4</v>
+      </c>
+      <c r="X8">
+        <v>9</v>
+      </c>
+      <c r="Y8">
+        <v>100</v>
+      </c>
+      <c r="Z8">
+        <v>9</v>
+      </c>
+      <c r="AA8">
+        <v>49</v>
+      </c>
+      <c r="AB8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AC8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9">
+        <v>846</v>
+      </c>
+      <c r="D9">
+        <v>873</v>
+      </c>
+      <c r="E9">
+        <v>895</v>
+      </c>
+      <c r="F9">
+        <v>869</v>
+      </c>
+      <c r="G9">
+        <v>854</v>
+      </c>
+      <c r="H9">
+        <v>3.2</v>
+      </c>
+      <c r="I9">
+        <v>2.5</v>
+      </c>
+      <c r="J9">
+        <v>-2.9000000000000004</v>
+      </c>
+      <c r="K9">
+        <v>-1.7000000000000002</v>
+      </c>
+      <c r="L9">
+        <v>12</v>
+      </c>
+      <c r="M9">
+        <v>11</v>
+      </c>
+      <c r="N9">
+        <v>8</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>9</v>
+      </c>
+      <c r="Q9">
+        <v>11</v>
+      </c>
+      <c r="R9">
+        <v>11</v>
+      </c>
+      <c r="S9">
+        <v>41.3</v>
+      </c>
+      <c r="T9">
+        <v>1822</v>
+      </c>
+      <c r="U9">
+        <v>331.5</v>
+      </c>
+      <c r="V9">
+        <v>124356</v>
+      </c>
+      <c r="W9">
+        <v>1000</v>
+      </c>
+      <c r="X9">
+        <v>9</v>
+      </c>
+      <c r="Y9">
+        <v>100</v>
+      </c>
+      <c r="Z9">
+        <v>9</v>
+      </c>
+      <c r="AA9">
+        <v>75</v>
+      </c>
+      <c r="AB9">
+        <v>9.6</v>
+      </c>
+      <c r="AC9">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10">
+        <v>786</v>
+      </c>
+      <c r="D10">
+        <v>783</v>
+      </c>
+      <c r="E10">
+        <v>809</v>
+      </c>
+      <c r="F10">
+        <v>800</v>
+      </c>
+      <c r="G10">
+        <v>793</v>
+      </c>
+      <c r="H10">
+        <v>-0.4</v>
+      </c>
+      <c r="I10">
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="J10">
+        <v>-1.0999999999999999</v>
+      </c>
+      <c r="K10">
+        <v>-0.89999999999999991</v>
+      </c>
+      <c r="L10">
+        <v>7</v>
+      </c>
+      <c r="M10">
+        <v>9</v>
+      </c>
+      <c r="N10">
+        <v>6</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <v>8</v>
+      </c>
+      <c r="Q10">
+        <v>3</v>
+      </c>
+      <c r="R10">
+        <v>6</v>
+      </c>
+      <c r="U10">
+        <v>372.6</v>
+      </c>
+      <c r="V10">
+        <v>36962</v>
+      </c>
+      <c r="W10">
+        <v>345.5</v>
+      </c>
+      <c r="X10">
+        <v>9.6</v>
+      </c>
+      <c r="Y10">
+        <v>100</v>
+      </c>
+      <c r="Z10">
+        <v>9.4</v>
+      </c>
+      <c r="AA10">
+        <v>30</v>
+      </c>
+      <c r="AB10">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AC10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11">
+        <v>880</v>
+      </c>
+      <c r="D11">
+        <v>908</v>
+      </c>
+      <c r="E11">
+        <v>899</v>
+      </c>
+      <c r="F11">
+        <v>893</v>
+      </c>
+      <c r="G11">
+        <v>921</v>
+      </c>
+      <c r="H11">
+        <v>3.2</v>
+      </c>
+      <c r="I11">
+        <v>-1</v>
+      </c>
+      <c r="J11">
+        <v>-0.70000000000000007</v>
+      </c>
+      <c r="K11">
+        <v>3.1</v>
+      </c>
+      <c r="L11">
+        <v>12</v>
+      </c>
+      <c r="M11">
+        <v>10</v>
+      </c>
+      <c r="N11">
+        <v>8</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>9</v>
+      </c>
+      <c r="Q11">
+        <v>11</v>
+      </c>
+      <c r="R11">
+        <v>11</v>
+      </c>
+      <c r="S11">
+        <v>55.8</v>
+      </c>
+      <c r="T11">
+        <v>1709</v>
+      </c>
+      <c r="U11">
+        <v>390.4</v>
+      </c>
+      <c r="V11">
+        <v>137761</v>
+      </c>
+      <c r="W11">
+        <v>864.3</v>
+      </c>
+      <c r="X11">
+        <v>9</v>
+      </c>
+      <c r="Y11">
+        <v>100</v>
+      </c>
+      <c r="Z11">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AA11">
+        <v>39</v>
+      </c>
+      <c r="AB11">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="AC11">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12">
+        <v>559</v>
+      </c>
+      <c r="D12">
+        <v>728</v>
+      </c>
+      <c r="E12">
+        <v>601</v>
+      </c>
+      <c r="F12">
+        <v>610</v>
+      </c>
+      <c r="G12">
+        <v>539</v>
+      </c>
+      <c r="H12">
+        <v>30.2</v>
+      </c>
+      <c r="I12">
+        <v>-17.399999999999999</v>
+      </c>
+      <c r="J12">
+        <v>1.5</v>
+      </c>
+      <c r="K12">
+        <v>-11.600000000000001</v>
+      </c>
+      <c r="L12">
+        <v>8</v>
+      </c>
+      <c r="M12">
+        <v>7</v>
+      </c>
+      <c r="N12">
+        <v>7</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>6</v>
+      </c>
+      <c r="Q12">
+        <v>11</v>
+      </c>
+      <c r="R12">
+        <v>11</v>
+      </c>
+      <c r="S12">
+        <v>47.4</v>
+      </c>
+      <c r="T12">
+        <v>1445</v>
+      </c>
+      <c r="U12">
+        <v>285.7</v>
+      </c>
+      <c r="V12">
+        <v>95114</v>
+      </c>
+      <c r="W12">
+        <v>669.2</v>
+      </c>
+      <c r="X12">
+        <v>9</v>
+      </c>
+      <c r="Y12">
+        <v>100</v>
+      </c>
+      <c r="Z12">
+        <v>8.6</v>
+      </c>
+      <c r="AA12">
+        <v>77</v>
+      </c>
+      <c r="AB12">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="AC12">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13">
+        <v>439</v>
+      </c>
+      <c r="D13">
+        <v>482</v>
+      </c>
+      <c r="E13">
+        <v>496</v>
+      </c>
+      <c r="F13">
+        <v>480</v>
+      </c>
+      <c r="G13">
+        <v>472</v>
+      </c>
+      <c r="H13">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I13">
+        <v>2.9000000000000004</v>
+      </c>
+      <c r="J13">
+        <v>-3.2</v>
+      </c>
+      <c r="K13">
+        <v>-1.7000000000000002</v>
+      </c>
+      <c r="L13">
+        <v>9</v>
+      </c>
+      <c r="M13">
+        <v>9</v>
+      </c>
+      <c r="N13">
+        <v>8</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>6</v>
+      </c>
+      <c r="Q13">
+        <v>11</v>
+      </c>
+      <c r="R13">
+        <v>11</v>
+      </c>
+      <c r="S13">
+        <v>56.6</v>
+      </c>
+      <c r="T13">
+        <v>1424</v>
+      </c>
+      <c r="U13">
+        <v>308.2</v>
+      </c>
+      <c r="V13">
+        <v>116090</v>
+      </c>
+      <c r="W13">
+        <v>672.4</v>
+      </c>
+      <c r="X13">
+        <v>10</v>
+      </c>
+      <c r="Y13">
+        <v>100</v>
+      </c>
+      <c r="Z13">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="AA13">
+        <v>59</v>
+      </c>
+      <c r="AB13">
+        <v>8.6</v>
+      </c>
+      <c r="AC13">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14">
+        <v>747</v>
+      </c>
+      <c r="D14">
+        <v>775</v>
+      </c>
+      <c r="E14">
+        <v>788</v>
+      </c>
+      <c r="F14">
+        <v>755</v>
+      </c>
+      <c r="G14">
+        <v>745</v>
+      </c>
+      <c r="H14">
+        <v>3.6999999999999997</v>
+      </c>
+      <c r="I14">
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="J14">
+        <v>-4.2</v>
+      </c>
+      <c r="K14">
+        <v>-1.3</v>
+      </c>
+      <c r="L14">
+        <v>9</v>
+      </c>
+      <c r="M14">
+        <v>12</v>
+      </c>
+      <c r="N14">
+        <v>7</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>6</v>
+      </c>
+      <c r="Q14">
+        <v>11</v>
+      </c>
+      <c r="R14">
+        <v>11</v>
+      </c>
+      <c r="S14">
+        <v>33</v>
+      </c>
+      <c r="T14">
+        <v>1302</v>
+      </c>
+      <c r="U14">
+        <v>1500</v>
+      </c>
+      <c r="V14">
+        <v>86758</v>
+      </c>
+      <c r="W14">
+        <v>3900</v>
+      </c>
+      <c r="X14">
+        <v>10</v>
+      </c>
+      <c r="Y14">
+        <v>100</v>
+      </c>
+      <c r="Z14">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AA14">
+        <v>100</v>
+      </c>
+      <c r="AB14">
+        <v>10</v>
+      </c>
+      <c r="AC14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15">
+        <v>190</v>
+      </c>
+      <c r="D15">
+        <v>188</v>
+      </c>
+      <c r="E15">
+        <v>190</v>
+      </c>
+      <c r="F15">
+        <v>179</v>
+      </c>
+      <c r="G15">
+        <v>179</v>
+      </c>
+      <c r="H15">
+        <v>-1.0999999999999999</v>
+      </c>
+      <c r="I15">
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="J15">
+        <v>-5.8000000000000007</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>12</v>
+      </c>
+      <c r="M15">
+        <v>12</v>
+      </c>
+      <c r="N15">
+        <v>8</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>9</v>
+      </c>
+      <c r="Q15">
+        <v>11</v>
+      </c>
+      <c r="R15">
+        <v>11</v>
+      </c>
+      <c r="S15">
+        <v>31.7</v>
+      </c>
+      <c r="T15">
+        <v>940</v>
+      </c>
+      <c r="U15">
+        <v>943.2</v>
+      </c>
+      <c r="V15">
+        <v>79344</v>
+      </c>
+      <c r="W15">
+        <v>2300</v>
+      </c>
+      <c r="X15">
+        <v>10</v>
+      </c>
+      <c r="Y15">
+        <v>100</v>
+      </c>
+      <c r="Z15">
+        <v>10</v>
+      </c>
+      <c r="AA15">
+        <v>100</v>
+      </c>
+      <c r="AB15">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AC15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16">
+        <v>523</v>
+      </c>
+      <c r="D16">
+        <v>519</v>
+      </c>
+      <c r="E16">
+        <v>527</v>
+      </c>
+      <c r="F16">
+        <v>509</v>
+      </c>
+      <c r="G16">
+        <v>499</v>
+      </c>
+      <c r="H16">
+        <v>-0.8</v>
+      </c>
+      <c r="I16">
+        <v>1.5</v>
+      </c>
+      <c r="J16">
+        <v>-3.4000000000000004</v>
+      </c>
+      <c r="K16">
+        <v>-2</v>
+      </c>
+      <c r="L16">
+        <v>12</v>
+      </c>
+      <c r="M16">
+        <v>12</v>
+      </c>
+      <c r="N16">
+        <v>9</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16">
+        <v>10</v>
+      </c>
+      <c r="Q16">
+        <v>11</v>
+      </c>
+      <c r="R16">
+        <v>9</v>
+      </c>
+      <c r="S16">
+        <v>61.7</v>
+      </c>
+      <c r="T16">
+        <v>1377</v>
+      </c>
+      <c r="U16">
+        <v>334.7</v>
+      </c>
+      <c r="V16">
+        <v>111232</v>
+      </c>
+      <c r="W16">
+        <v>688.2</v>
+      </c>
+      <c r="X16">
+        <v>9.4</v>
+      </c>
+      <c r="Y16">
+        <v>91</v>
+      </c>
+      <c r="Z16">
+        <v>8</v>
+      </c>
+      <c r="AA16">
+        <v>32</v>
+      </c>
+      <c r="AB16">
+        <v>8.4</v>
+      </c>
+      <c r="AC16">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>76</v>
+      </c>
+      <c r="R1" t="s">
+        <v>77</v>
+      </c>
+      <c r="S1" t="s">
+        <v>118</v>
+      </c>
+      <c r="T1" t="s">
+        <v>119</v>
+      </c>
+      <c r="U1" t="s">
+        <v>120</v>
+      </c>
+      <c r="V1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2">
+        <v>171</v>
+      </c>
+      <c r="D2">
+        <v>183</v>
+      </c>
+      <c r="E2">
+        <v>187</v>
+      </c>
+      <c r="F2">
+        <v>184</v>
+      </c>
+      <c r="G2">
+        <v>182</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2:K14" si="0">ROUND((D2-C2)/C2,3)</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>-1.6E-2</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="0"/>
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="L2">
+        <v>12</v>
+      </c>
+      <c r="M2">
+        <v>11</v>
+      </c>
+      <c r="N2">
+        <v>8</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+      <c r="P2">
+        <v>9</v>
+      </c>
+      <c r="Q2">
+        <v>7</v>
+      </c>
+      <c r="R2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3">
+        <v>161</v>
+      </c>
+      <c r="D3">
+        <v>88</v>
+      </c>
+      <c r="E3">
+        <v>93</v>
+      </c>
+      <c r="F3">
+        <v>80</v>
+      </c>
+      <c r="G3">
+        <v>75</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>-0.45300000000000001</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>-6.3E-2</v>
+      </c>
+      <c r="L3">
+        <v>12</v>
+      </c>
+      <c r="M3">
+        <v>12</v>
+      </c>
+      <c r="N3">
+        <v>7</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <v>9</v>
+      </c>
+      <c r="Q3">
+        <v>11</v>
+      </c>
+      <c r="R3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4">
+        <v>236</v>
+      </c>
+      <c r="D4">
+        <v>241</v>
+      </c>
+      <c r="E4">
+        <v>233</v>
+      </c>
+      <c r="F4">
+        <v>220</v>
+      </c>
+      <c r="G4">
+        <v>218</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>-3.3000000000000002E-2</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>-5.6000000000000001E-2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>-8.9999999999999993E-3</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>12</v>
+      </c>
+      <c r="N4">
+        <v>9</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <v>6</v>
+      </c>
+      <c r="Q4">
+        <v>11</v>
+      </c>
+      <c r="R4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5">
+        <v>350</v>
+      </c>
+      <c r="D5">
+        <v>395</v>
+      </c>
+      <c r="E5">
+        <v>376</v>
+      </c>
+      <c r="F5">
+        <v>355</v>
+      </c>
+      <c r="G5">
+        <v>347</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0.129</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>-4.8000000000000001E-2</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>-5.6000000000000001E-2</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>-2.3E-2</v>
+      </c>
+      <c r="L5">
+        <v>12</v>
+      </c>
+      <c r="M5">
+        <v>12</v>
+      </c>
+      <c r="N5">
+        <v>9</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>10</v>
+      </c>
+      <c r="Q5">
+        <v>11</v>
+      </c>
+      <c r="R5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6">
+        <v>174</v>
+      </c>
+      <c r="D6">
+        <v>187</v>
+      </c>
+      <c r="E6">
+        <v>184</v>
+      </c>
+      <c r="F6">
+        <v>175</v>
+      </c>
+      <c r="G6">
+        <v>173</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>-1.6E-2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="L6">
+        <v>12</v>
+      </c>
+      <c r="M6">
+        <v>12</v>
+      </c>
+      <c r="N6">
+        <v>7</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <v>9</v>
+      </c>
+      <c r="Q6">
+        <v>11</v>
+      </c>
+      <c r="R6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>